<commit_message>
Ajustes moldes backend y fronted
</commit_message>
<xml_diff>
--- a/planning/assets/formatsXlsx/Productos.xlsx
+++ b/planning/assets/formatsXlsx/Productos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>referencia</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>cantidad</t>
+  </si>
+  <si>
+    <t>molde</t>
   </si>
 </sst>
 </file>
@@ -142,7 +145,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -166,13 +169,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -312,11 +332,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:C6" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
-  <tableColumns count="3">
-    <tableColumn id="1" name="referencia" dataDxfId="2"/>
-    <tableColumn id="2" name="producto" dataDxfId="1"/>
-    <tableColumn id="3" name="cantidad" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:D6" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <tableColumns count="4">
+    <tableColumn id="1" name="referencia" dataDxfId="3"/>
+    <tableColumn id="2" name="producto" dataDxfId="2"/>
+    <tableColumn id="3" name="molde" dataDxfId="1"/>
+    <tableColumn id="4" name="cantidad" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -607,20 +628,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="47.85546875" customWidth="1"/>
     <col min="2" max="2" width="50.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
+    <row r="1" spans="1:4" ht="18">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -628,33 +650,41 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="6"/>
+      <c r="D2" s="9"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" s="1"/>
       <c r="B3" s="3"/>
       <c r="C3" s="7"/>
+      <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" s="1"/>
       <c r="B4" s="3"/>
       <c r="C4" s="7"/>
+      <c r="D4" s="9"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5" s="1"/>
       <c r="B5" s="3"/>
       <c r="C5" s="7"/>
+      <c r="D5" s="9"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6" s="1"/>
       <c r="B6" s="3"/>
       <c r="C6" s="8"/>
+      <c r="D6" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Creacion ventas Backend y Fronted
</commit_message>
<xml_diff>
--- a/planning/assets/formatsXlsx/Productos.xlsx
+++ b/planning/assets/formatsXlsx/Productos.xlsx
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>referencia</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>producto</t>
   </si>
@@ -27,12 +24,18 @@
   <si>
     <t>molde</t>
   </si>
+  <si>
+    <t>referencia_producto</t>
+  </si>
+  <si>
+    <t>referencia_molde</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -51,6 +54,16 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -145,7 +158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -172,13 +185,49 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -332,12 +381,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:D6" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <tableColumns count="4">
-    <tableColumn id="1" name="referencia" dataDxfId="3"/>
-    <tableColumn id="2" name="producto" dataDxfId="2"/>
-    <tableColumn id="3" name="molde" dataDxfId="1"/>
-    <tableColumn id="4" name="cantidad" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:E6" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+  <tableColumns count="5">
+    <tableColumn id="1" name="referencia_producto" dataDxfId="4"/>
+    <tableColumn id="2" name="producto" dataDxfId="3"/>
+    <tableColumn id="3" name="referencia_molde" dataDxfId="2"/>
+    <tableColumn id="4" name="molde" dataDxfId="1"/>
+    <tableColumn id="5" name="cantidad" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -628,63 +678,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="47.85546875" customWidth="1"/>
     <col min="2" max="2" width="50.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18">
+    <row r="1" spans="1:5" ht="18">
       <c r="A1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="10" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="6"/>
       <c r="D2" s="9"/>
+      <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" s="1"/>
       <c r="B3" s="3"/>
       <c r="C3" s="7"/>
       <c r="D3" s="9"/>
+      <c r="E3" s="12"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" s="1"/>
       <c r="B4" s="3"/>
       <c r="C4" s="7"/>
       <c r="D4" s="9"/>
+      <c r="E4" s="12"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5" s="1"/>
       <c r="B5" s="3"/>
       <c r="C5" s="7"/>
       <c r="D5" s="9"/>
+      <c r="E5" s="12"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5">
       <c r="A6" s="1"/>
       <c r="B6" s="3"/>
       <c r="C6" s="8"/>
       <c r="D6" s="9"/>
+      <c r="E6" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Crecion productos en proceso, planeacion
</commit_message>
<xml_diff>
--- a/planning/assets/formatsXlsx/Productos.xlsx
+++ b/planning/assets/formatsXlsx/Productos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Ledesma\Documents\Documentos\teenus\importaciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F79FA9D-6B47-4D19-A4D4-54ABB733455A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40EBA83E-86AE-4E32-8444-91CD35938D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>producto</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>cantidad_producto</t>
+  </si>
+  <si>
+    <t>categoria</t>
   </si>
 </sst>
 </file>
@@ -64,12 +67,14 @@
     <font>
       <sz val="12"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -177,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -210,13 +215,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="11">
     <dxf>
       <font>
         <strike val="0"/>
@@ -230,18 +241,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -317,6 +316,32 @@
         </right>
         <top/>
         <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -420,13 +445,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A1:E5" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="referencia_producto" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="producto" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="cantidad_producto" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A1:F5" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="referencia_producto" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="producto" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="cantidad_producto" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="referencia_molde" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="molde" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{3ABAFBF7-26A8-4DD6-B6B3-F1992B17FBC1}" name="categoria" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -753,10 +779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,11 +790,12 @@
     <col min="1" max="1" width="40.28515625" customWidth="1"/>
     <col min="2" max="2" width="40.140625" customWidth="1"/>
     <col min="3" max="3" width="34.28515625" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -784,34 +811,41 @@
       <c r="E1" s="9" t="s">
         <v>1</v>
       </c>
+      <c r="F1" s="13" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="11"/>
       <c r="D2" s="8"/>
       <c r="E2" s="6"/>
+      <c r="F2" s="12"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="6"/>
       <c r="D3" s="8"/>
       <c r="E3" s="6"/>
+      <c r="F3" s="12"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="6"/>
       <c r="D4" s="8"/>
       <c r="E4" s="6"/>
+      <c r="F4" s="12"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="5"/>
       <c r="C5" s="10"/>
       <c r="D5" s="8"/>
       <c r="E5" s="10"/>
+      <c r="F5" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ajustes productos en proceso, planeacion
</commit_message>
<xml_diff>
--- a/planning/assets/formatsXlsx/Productos.xlsx
+++ b/planning/assets/formatsXlsx/Productos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Ledesma\Documents\Documentos\teenus\importaciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40EBA83E-86AE-4E32-8444-91CD35938D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D252526-352E-4870-A947-0AA2C4F790F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,6 +76,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -85,7 +91,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -147,17 +153,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -182,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -196,31 +191,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -238,9 +224,21 @@
         <sz val="12"/>
         <color auto="1"/>
         <name val="Arial"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -445,14 +443,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A1:F5" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A1:F6" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="referencia_producto" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="producto" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{3ABAFBF7-26A8-4DD6-B6B3-F1992B17FBC1}" name="categoria" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="cantidad_producto" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="referencia_molde" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="molde" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{3ABAFBF7-26A8-4DD6-B6B3-F1992B17FBC1}" name="categoria" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -779,10 +777,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,7 +789,7 @@
     <col min="2" max="2" width="40.140625" customWidth="1"/>
     <col min="3" max="3" width="34.28515625" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" customWidth="1"/>
     <col min="6" max="6" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -799,55 +797,64 @@
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="7" t="s">
         <v>1</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
-      <c r="C2" s="11"/>
+      <c r="C2" s="9"/>
       <c r="D2" s="8"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="12"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="12"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="9"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="12"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="9"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="12"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="9"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="9"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>